<commit_message>
changes from other branches
</commit_message>
<xml_diff>
--- a/Data/Excels/Elastic_TwoPoints_1.xlsx
+++ b/Data/Excels/Elastic_TwoPoints_1.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>InRays</t>
+          <t>{'TwoPoints'}</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -830,17 +830,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1,16</t>
+          <t>1,53</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1,22</t>
+          <t>1,53</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1,15e-03</t>
+          <t>8,37e-05</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -876,12 +876,12 @@
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>3,26</t>
+          <t>3,34</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>3,97</t>
+          <t>4,03</t>
         </is>
       </c>
       <c r="R6" t="inlineStr"/>
@@ -915,17 +915,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0,99</t>
+          <t>0,97</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1,03</t>
+          <t>1,01</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2,54e-03</t>
+          <t>2,59e-03</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>-0,0</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -961,12 +961,12 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
-          <t>3,23</t>
+          <t>3,22</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>3,96</t>
+          <t>3,95</t>
         </is>
       </c>
       <c r="R7" t="inlineStr"/>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0,98</t>
+          <t>0,99</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2,75e-03</t>
+          <t>2,72e-03</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>-0,0</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1085,17 +1085,17 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0,99</t>
+          <t>1,01</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1,02</t>
+          <t>1,04</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2,98e-03</t>
+          <t>2,67e-03</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>-0,0</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0,98</t>
+          <t>0,99</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>3,05e-03</t>
+          <t>2,96e-03</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>-0,0</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1225,17 +1225,17 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>3,98</t>
+          <t>3,99</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>3,43</t>
+          <t>3,33</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>82,49</t>
+          <t>82,57</t>
         </is>
       </c>
     </row>
@@ -1267,17 +1267,17 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>0,94</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>0,92</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>6,41e-04</t>
+          <t>0,00e+00</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1317,12 +1317,12 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>1,51</t>
+          <t>1,64</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>1,72</t>
+          <t>1,82</t>
         </is>
       </c>
       <c r="R11" t="inlineStr"/>
@@ -1356,17 +1356,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0,25</t>
+          <t>0,92</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0,25</t>
+          <t>0,91</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1,80e-04</t>
+          <t>7,28e-08</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1402,12 +1402,12 @@
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
-          <t>1,48</t>
+          <t>1,64</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>1,68</t>
+          <t>1,81</t>
         </is>
       </c>
       <c r="R12" t="inlineStr"/>
@@ -1441,17 +1441,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0,29</t>
+          <t>0,92</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0,29</t>
+          <t>0,91</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1,29e-04</t>
+          <t>7,84e-08</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1487,12 +1487,12 @@
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
         <is>
-          <t>1,47</t>
+          <t>1,64</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>1,68</t>
+          <t>1,81</t>
         </is>
       </c>
       <c r="R13" t="inlineStr"/>
@@ -1526,17 +1526,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0,32</t>
+          <t>0,92</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0,32</t>
+          <t>0,90</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>9,80e-05</t>
+          <t>9,41e-08</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1572,12 +1572,12 @@
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
-          <t>1,46</t>
+          <t>1,64</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>1,67</t>
+          <t>1,81</t>
         </is>
       </c>
       <c r="R14" t="inlineStr"/>
@@ -1611,17 +1611,17 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0,35</t>
+          <t>0,92</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0,35</t>
+          <t>0,90</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>7,56e-05</t>
+          <t>9,32e-08</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1657,12 +1657,12 @@
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr">
         <is>
-          <t>1,46</t>
+          <t>1,64</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>1,67</t>
+          <t>1,81</t>
         </is>
       </c>
       <c r="R15" t="inlineStr"/>
@@ -1696,17 +1696,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0,37</t>
+          <t>0,92</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0,37</t>
+          <t>0,90</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>6,22e-05</t>
+          <t>7,65e-08</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1746,22 +1746,22 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>1,46</t>
+          <t>1,64</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>1,67</t>
+          <t>1,81</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>3,84</t>
+          <t>0,44</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>58,26</t>
+          <t>65,42</t>
         </is>
       </c>
     </row>
@@ -1793,17 +1793,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>2,21</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4,74</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1,03e-02</t>
+          <t>0,00e+00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1843,12 +1843,12 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>3,17</t>
+          <t>3,49</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>3,90</t>
+          <t>4,12</t>
         </is>
       </c>
       <c r="R17" t="inlineStr"/>
@@ -1882,17 +1882,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1,30</t>
+          <t>2,26</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0,80</t>
+          <t>2,32</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>3,95e-03</t>
+          <t>4,94e-05</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>-0,0</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1928,12 +1928,12 @@
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr">
         <is>
-          <t>3,29</t>
+          <t>3,46</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>3,98</t>
+          <t>4,10</t>
         </is>
       </c>
       <c r="R18" t="inlineStr"/>
@@ -1967,17 +1967,17 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1,28</t>
+          <t>2,20</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0,78</t>
+          <t>1,80</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>4,12e-03</t>
+          <t>3,05e-04</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>-0,0</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -2013,12 +2013,12 @@
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t>3,30</t>
+          <t>3,43</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>3,98</t>
+          <t>4,07</t>
         </is>
       </c>
       <c r="R19" t="inlineStr"/>
@@ -2052,17 +2052,17 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1,29</t>
+          <t>1,97</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0,80</t>
+          <t>1,39</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>4,15e-03</t>
+          <t>1,08e-03</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>-0,0</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -2098,12 +2098,12 @@
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t>3,31</t>
+          <t>3,37</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>3,99</t>
+          <t>4,03</t>
         </is>
       </c>
       <c r="R20" t="inlineStr"/>
@@ -2137,17 +2137,17 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>1,27</t>
+          <t>1,94</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0,79</t>
+          <t>1,31</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>4,37e-03</t>
+          <t>1,38e-03</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>-0,0</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -2183,12 +2183,12 @@
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t>3,31</t>
+          <t>3,37</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>3,99</t>
+          <t>4,02</t>
         </is>
       </c>
       <c r="R21" t="inlineStr"/>
@@ -2222,17 +2222,17 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1,27</t>
+          <t>1,93</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0,79</t>
+          <t>1,28</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>4,44e-03</t>
+          <t>1,50e-03</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2252,19 +2252,19 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
+          <t>0,0</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>0,0</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
           <t>-0,0</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>0,0</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>-0,0</t>
-        </is>
-      </c>
       <c r="O22" t="inlineStr">
         <is>
           <t>4,73</t>
@@ -2272,22 +2272,22 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>3,31</t>
+          <t>3,37</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>4,00</t>
+          <t>4,03</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>-4,57</t>
+          <t>3,52</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>70,13</t>
+          <t>71,25</t>
         </is>
       </c>
     </row>
@@ -2319,17 +2319,17 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7,13</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>6,99</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1,58e-01</t>
+          <t>0,00e+00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2369,12 +2369,12 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>12,24</t>
+          <t>13,77</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>15,41</t>
+          <t>16,32</t>
         </is>
       </c>
       <c r="R23" t="inlineStr"/>
@@ -2408,17 +2408,17 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0,81</t>
+          <t>6,93</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0,93</t>
+          <t>6,82</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1,49e-01</t>
+          <t>9,53e-05</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2454,12 +2454,12 @@
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr">
         <is>
-          <t>13,50</t>
+          <t>13,72</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>16,95</t>
+          <t>16,28</t>
         </is>
       </c>
       <c r="R24" t="inlineStr"/>
@@ -2493,17 +2493,17 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0,96</t>
+          <t>6,24</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1,05</t>
+          <t>6,19</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1,47e-01</t>
+          <t>2,08e-03</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2539,12 +2539,12 @@
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr">
         <is>
-          <t>13,75</t>
+          <t>13,53</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>17,31</t>
+          <t>16,16</t>
         </is>
       </c>
       <c r="R25" t="inlineStr"/>
@@ -2578,17 +2578,17 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0,96</t>
+          <t>5,29</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1,14</t>
+          <t>5,28</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1,55e-01</t>
+          <t>1,15e-02</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>-0,0</t>
+          <t>-0,01</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -2624,12 +2624,12 @@
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr">
         <is>
-          <t>13,95</t>
+          <t>13,28</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>17,71</t>
+          <t>16,00</t>
         </is>
       </c>
       <c r="R26" t="inlineStr"/>
@@ -2663,17 +2663,17 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0,90</t>
+          <t>5,12</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1,02</t>
+          <t>5,07</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1,48e-01</t>
+          <t>1,55e-02</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2698,7 +2698,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>-0,0</t>
+          <t>-0,01</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -2709,12 +2709,12 @@
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr">
         <is>
-          <t>14,38</t>
+          <t>13,24</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>18,27</t>
+          <t>15,97</t>
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
@@ -2748,17 +2748,17 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1,07</t>
+          <t>5,05</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>1,06</t>
+          <t>5,03</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1,56e-01</t>
+          <t>1,76e-02</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2783,14 +2783,14 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
+          <t>-0,01</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
           <t>-0,0</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>-0,0</t>
-        </is>
-      </c>
       <c r="O28" t="inlineStr">
         <is>
           <t>16,05</t>
@@ -2798,22 +2798,22 @@
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>14,85</t>
+          <t>13,22</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>18,95</t>
+          <t>15,97</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>-21,36</t>
+          <t>3,99</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>92,49</t>
+          <t>82,37</t>
         </is>
       </c>
     </row>
@@ -2845,17 +2845,17 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,49</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>3,41</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1,10e-03</t>
+          <t>0,00e+00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2895,12 +2895,12 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>4,65</t>
+          <t>5,57</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>5,39</t>
+          <t>6,02</t>
         </is>
       </c>
       <c r="R29" t="inlineStr"/>
@@ -2934,17 +2934,17 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0,54</t>
+          <t>2,62</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0,49</t>
+          <t>2,58</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>3,99e-04</t>
+          <t>2,11e-05</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2974,18 +2974,18 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>-0,0</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t>4,58</t>
+          <t>5,22</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>5,32</t>
+          <t>5,75</t>
         </is>
       </c>
       <c r="R30" t="inlineStr"/>
@@ -3019,17 +3019,17 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>0,62</t>
+          <t>0,95</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>0,55</t>
+          <t>0,94</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>3,56e-04</t>
+          <t>2,43e-04</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -3054,23 +3054,23 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
+          <t>0,01</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
           <t>0,0</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>-0,0</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t>4,57</t>
+          <t>4,72</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>5,32</t>
+          <t>5,42</t>
         </is>
       </c>
       <c r="R31" t="inlineStr"/>
@@ -3104,17 +3104,17 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>0,68</t>
+          <t>0,97</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0,61</t>
+          <t>0,96</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>3,33e-04</t>
+          <t>2,08e-04</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -3139,23 +3139,23 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
+          <t>0,02</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
           <t>0,0</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>-0,0</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t>4,56</t>
+          <t>4,72</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>5,31</t>
+          <t>5,42</t>
         </is>
       </c>
       <c r="R32" t="inlineStr"/>
@@ -3189,17 +3189,17 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0,71</t>
+          <t>0,98</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0,62</t>
+          <t>0,98</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>3,23e-04</t>
+          <t>1,89e-04</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -3224,23 +3224,23 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
+          <t>0,02</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
           <t>0,0</t>
-        </is>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>-0,0</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t>4,55</t>
+          <t>4,72</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>5,30</t>
+          <t>5,42</t>
         </is>
       </c>
       <c r="R33" t="inlineStr"/>
@@ -3274,17 +3274,17 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0,71</t>
+          <t>0,98</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>0,62</t>
+          <t>0,98</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>3,20e-04</t>
+          <t>1,83e-04</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -3309,14 +3309,14 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
+          <t>0,03</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
           <t>0,0</t>
         </is>
       </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>-0,0</t>
-        </is>
-      </c>
       <c r="O34" t="inlineStr">
         <is>
           <t>10,00</t>
@@ -3324,22 +3324,22 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>4,54</t>
+          <t>4,72</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>5,30</t>
+          <t>5,42</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>2,31</t>
+          <t>15,27</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>45,44</t>
+          <t>47,20</t>
         </is>
       </c>
     </row>
@@ -3371,17 +3371,17 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>8,23</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>8,13</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1,79e-01</t>
+          <t>0,00e+00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -3421,12 +3421,12 @@
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>12,90</t>
+          <t>14,59</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>16,37</t>
+          <t>17,47</t>
         </is>
       </c>
       <c r="R35" t="inlineStr"/>
@@ -3460,17 +3460,17 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>6,92</t>
+          <t>7,87</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>12,98</t>
+          <t>7,75</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2,58e-02</t>
+          <t>1,70e-04</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -3506,12 +3506,12 @@
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
-          <t>13,80</t>
+          <t>14,48</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>16,61</t>
+          <t>17,39</t>
         </is>
       </c>
       <c r="R36" t="inlineStr"/>
@@ -3545,17 +3545,17 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>6,46</t>
+          <t>7,03</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>12,64</t>
+          <t>6,90</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1,17e-02</t>
+          <t>2,22e-03</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,01</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
@@ -3591,12 +3591,12 @@
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
-          <t>13,57</t>
+          <t>14,24</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>16,44</t>
+          <t>17,21</t>
         </is>
       </c>
       <c r="R37" t="inlineStr"/>
@@ -3630,17 +3630,17 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>5,28</t>
+          <t>6,07</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>10,13</t>
+          <t>5,97</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1,12e-02</t>
+          <t>9,92e-03</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -3665,7 +3665,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,01</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -3676,12 +3676,12 @@
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr">
         <is>
-          <t>13,16</t>
+          <t>13,98</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>16,11</t>
+          <t>17,02</t>
         </is>
       </c>
       <c r="R38" t="inlineStr"/>
@@ -3715,17 +3715,17 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>4,94</t>
+          <t>5,99</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>9,69</t>
+          <t>5,85</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1,21e-02</t>
+          <t>1,12e-02</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,02</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
@@ -3761,12 +3761,12 @@
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr">
         <is>
-          <t>13,04</t>
+          <t>13,95</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>16,02</t>
+          <t>17,00</t>
         </is>
       </c>
       <c r="R39" t="inlineStr"/>
@@ -3800,17 +3800,17 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>4,33</t>
+          <t>5,98</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>6,98</t>
+          <t>5,83</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2,45e-02</t>
+          <t>1,12e-02</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,02</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -3850,22 +3850,22 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>12,91</t>
+          <t>13,95</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>15,90</t>
+          <t>17,00</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>-0,10</t>
+          <t>4,38</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>67,47</t>
+          <t>72,86</t>
         </is>
       </c>
     </row>
@@ -3897,17 +3897,17 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,66</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>1,59</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1,02e-03</t>
+          <t>0,00e+00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -3947,12 +3947,12 @@
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>1,73</t>
+          <t>2,03</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>2,09</t>
+          <t>2,45</t>
         </is>
       </c>
       <c r="R41" t="inlineStr"/>
@@ -3986,17 +3986,17 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0,41</t>
+          <t>1,61</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>0,41</t>
+          <t>1,56</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>4,40e-04</t>
+          <t>3,76e-07</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -4032,12 +4032,12 @@
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t>1,56</t>
+          <t>2,01</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>1,90</t>
+          <t>2,43</t>
         </is>
       </c>
       <c r="R42" t="inlineStr"/>
@@ -4071,17 +4071,17 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0,46</t>
+          <t>1,47</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>0,45</t>
+          <t>1,45</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>4,09e-04</t>
+          <t>6,32e-06</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -4117,12 +4117,12 @@
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t>1,55</t>
+          <t>1,97</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>1,89</t>
+          <t>2,38</t>
         </is>
       </c>
       <c r="R43" t="inlineStr"/>
@@ -4156,17 +4156,17 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0,51</t>
+          <t>1,03</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>0,49</t>
+          <t>1,09</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>3,96e-04</t>
+          <t>7,45e-05</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -4202,12 +4202,12 @@
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr">
         <is>
-          <t>1,55</t>
+          <t>1,85</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>1,88</t>
+          <t>2,24</t>
         </is>
       </c>
       <c r="R44" t="inlineStr"/>
@@ -4241,17 +4241,17 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0,55</t>
+          <t>0,98</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>0,51</t>
+          <t>1,04</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>3,91e-04</t>
+          <t>8,39e-05</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -4287,12 +4287,12 @@
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t>1,54</t>
+          <t>1,83</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>1,87</t>
+          <t>2,22</t>
         </is>
       </c>
       <c r="R45" t="inlineStr"/>
@@ -4326,17 +4326,17 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0,56</t>
+          <t>0,97</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>0,52</t>
+          <t>1,03</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>3,91e-04</t>
+          <t>8,41e-05</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -4376,22 +4376,22 @@
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>1,53</t>
+          <t>1,83</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>1,86</t>
+          <t>2,21</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>11,51</t>
+          <t>9,87</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>47,36</t>
+          <t>56,49</t>
         </is>
       </c>
     </row>

</xml_diff>